<commit_message>
Removed functions from all_city_for_Chris
</commit_message>
<xml_diff>
--- a/all_city_for_Chris.xlsx
+++ b/all_city_for_Chris.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kailyn Hogan\OneDrive - Iowa State University\Documents\GitHub\Housing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C902AA82-B565-48D7-B2D8-64EFECD45499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C2993-E021-4884-BA1D-3FC1B8076147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="325">
   <si>
     <t>Parcel ID</t>
   </si>
@@ -431,6 +431,600 @@
   </si>
   <si>
     <t>URL Address</t>
+  </si>
+  <si>
+    <t>G_I_2094 JAMESTOWN AVE.png</t>
+  </si>
+  <si>
+    <t>G_I_1403 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1500 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1402 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1501 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1500 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1502 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1503 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_502 14TH ST NE.png</t>
+  </si>
+  <si>
+    <t>G_I_504 14TH ST NE.png</t>
+  </si>
+  <si>
+    <t>G_I_600 14TH ST NE.png</t>
+  </si>
+  <si>
+    <t>G_I_602 14TH ST NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1501 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1502 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1504 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1503 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1504 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1506 NORTH RIDGE CT NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1505 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1506 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_1803 8TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_2089 KENTUCKY AVE.png</t>
+  </si>
+  <si>
+    <t>G_I_1508 6TH AVE NE.png</t>
+  </si>
+  <si>
+    <t>G_I_502 16TH ST NE.png</t>
+  </si>
+  <si>
+    <t>G_H_116 N CHESTNUT ST.png</t>
+  </si>
+  <si>
+    <t>G_H_12 E COURT ST.png</t>
+  </si>
+  <si>
+    <t>G_H_311 W MAIN ST.png</t>
+  </si>
+  <si>
+    <t>G_H_102 E MAIN ST.png</t>
+  </si>
+  <si>
+    <t>G_H_508 N LINN AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_9 W GARDNER ST.png</t>
+  </si>
+  <si>
+    <t>G_H_7 W COURT ST.png</t>
+  </si>
+  <si>
+    <t>G_H_213 N WALNUT AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_22 N LINN AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_316 N WALNUT AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_14 E WASHINGTON ST.png</t>
+  </si>
+  <si>
+    <t>G_H_311 N LOCUST AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_101 N LOCUST AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_615 N LINN AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_206 N FOLEY AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_214 E WASHINGTON ST.png</t>
+  </si>
+  <si>
+    <t>G_H_206 N LINN AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_102 N LINN AVE.png</t>
+  </si>
+  <si>
+    <t>G_H_313 E MILWAUKEE ST.png</t>
+  </si>
+  <si>
+    <t>G_H_4 E HALE ST.png</t>
+  </si>
+  <si>
+    <t>G_H_104 E MAIN ST.png</t>
+  </si>
+  <si>
+    <t>G_H_602 HOMESTEAD CIR.png</t>
+  </si>
+  <si>
+    <t>G_H_607 HOMESTEAD CIR.png</t>
+  </si>
+  <si>
+    <t>G_H_616 HOMESTEAD CIR.png</t>
+  </si>
+  <si>
+    <t>G_H_601 HOMESTEAD CIR.png</t>
+  </si>
+  <si>
+    <t>G_S_ 701 BENTON CIR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 637 GREENE ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 705 TAMA CIR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 608 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 604 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 202 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 104 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 706 MARSHALL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 900 FOUR MILE DR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 638 GREENE ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 700 TAMA CIR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 705 BENTON CIR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 700 BENTON CIR .png</t>
+  </si>
+  <si>
+    <t>G_S_ 610 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 204 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 614 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 708 MARSHALL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 101 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 100 8TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 305 9TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_S_ 804 S CARROLL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 605 MARSHALL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 807 S CARROLL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 811 S CARROLL ST .png</t>
+  </si>
+  <si>
+    <t>G_S_ 108 10TH AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 303 I AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 301 I AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 1206 4TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 505 I AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 212 K AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 1208 5TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 808 FROST ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 307 I AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 310 E M Ave.png</t>
+  </si>
+  <si>
+    <t>G_D_ 501 HYDE AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 302 H AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 314 H AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 411 Hyde Ave.png</t>
+  </si>
+  <si>
+    <t>G_D_ 403 H AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 708 5TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 302 E H AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 310 G AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 1204 4TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 1202 4TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 803 FROST ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 1104 4TH ST .png</t>
+  </si>
+  <si>
+    <t>G_D_ 212 J AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 202 K AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 313 H AVE .png</t>
+  </si>
+  <si>
+    <t>G_D_ 502 BUTLER AVE .png</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=2094+JAMESTOWN+AVE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1403+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1500+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1402+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1501+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1500+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1502+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1503+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+14TH+ST+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=504+14TH+ST+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=600+14TH+ST+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=602+14TH+ST+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1501+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1502+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1504+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1503+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1504+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1506+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1505+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1506+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1803+8TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=2089+KENTUCKY+AVE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1508+6TH+AVE+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+16TH+ST+NE,INDEPENDENCE+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=116+N+CHESTNUT+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=12+E+COURT+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=311+W+MAIN+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=102+E+MAIN+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=508+N+LINN+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=9+W+GARDNER+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=7+W+COURT+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=213+N+WALNUT+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=22+N+LINN+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=316+N+WALNUT+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=14+E+WASHINGTON+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=311+N+LOCUST+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=101+N+LOCUST+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=615+N+LINN+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=206+N+FOLEY+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=214+E+WASHINGTON+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=206+N+LINN+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=102+N+LINN+AVE,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=313+E+MILWAUKEE+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=4+E+HALE+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=104+E+MAIN+ST,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=602+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=607+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=616+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=601+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=701+BENTON+CIR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=637+GREENE+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=705+TAMA+CIR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=608+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=604+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=202+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=104+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=706+MARSHALL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=900+FOUR+MILE+DR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=638+GREENE+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=700+TAMA+CIR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=705+BENTON+CIR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=700+BENTON+CIR,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=610+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=204+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=614+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=708+MARSHALL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=101+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=100+8TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=305+9TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=804+S+CARROLL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=605+MARSHALL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=807+S+CARROLL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=811+S+CARROLL+ST,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=108+10TH+AVE,SLATER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=303+I+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=301+I+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1206+4TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=505+I+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=212+K+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1208+5TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=808+FROST+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=307+I+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=310+E+M+Ave,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=501+HYDE+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=302+H+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=314+H+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=411+Hyde+Ave,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=403+H+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=708+5TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=302+E+H+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=310+G+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1204+4TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1202+4TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=803+FROST+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1104+4TH+ST,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=212+J+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=202+K+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=313+H+AVE,GRUNDY+CENTER+IOWA</t>
+  </si>
+  <si>
+    <t>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+BUTLER+AVE,GRUNDY+CENTER+IOWA</t>
   </si>
 </sst>
 </file>
@@ -758,7 +1352,7 @@
   <dimension ref="A1:V101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -854,16 +1448,14 @@
         <v>124</v>
       </c>
       <c r="E2" t="str">
-        <f>IF(LEFT(H2,1)="I","I",IF(LEFT(H2,1)="S","S",IF(LEFT(H2,1)="N","H",IF(LEFT(H2,1)="G","D"))))</f>
+        <f t="shared" ref="E2:E33" si="0">IF(LEFT(H2,1)="I","I",IF(LEFT(H2,1)="S","S",IF(LEFT(H2,1)="N","H",IF(LEFT(H2,1)="G","D"))))</f>
         <v>I</v>
       </c>
-      <c r="F2" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B2),",",H2," ",C2)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=2094+JAMESTOWN+AVE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G2" t="str">
-        <f>CONCATENATE(D2,"_",E2,"_",B2,".png")</f>
-        <v>G_I_2094 JAMESTOWN AVE.png</v>
+      <c r="F2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" t="s">
+        <v>127</v>
       </c>
       <c r="H2" t="s">
         <v>79</v>
@@ -883,16 +1475,14 @@
         <v>124</v>
       </c>
       <c r="E3" t="str">
-        <f>IF(LEFT(H3,1)="I","I",IF(LEFT(H3,1)="S","S",IF(LEFT(H3,1)="N","H",IF(LEFT(H3,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F3" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B3),",",H3," ",C3)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1403+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G3" t="str">
-        <f>CONCATENATE(D3,"_",E3,"_",B3,".png")</f>
-        <v>G_I_1403 6TH AVE NE.png</v>
+      <c r="F3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" t="s">
+        <v>128</v>
       </c>
       <c r="H3" t="s">
         <v>79</v>
@@ -912,16 +1502,14 @@
         <v>124</v>
       </c>
       <c r="E4" t="str">
-        <f>IF(LEFT(H4,1)="I","I",IF(LEFT(H4,1)="S","S",IF(LEFT(H4,1)="N","H",IF(LEFT(H4,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F4" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B4),",",H4," ",C4)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1500+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G4" t="str">
-        <f>CONCATENATE(D4,"_",E4,"_",B4,".png")</f>
-        <v>G_I_1500 NORTH RIDGE CT NE.png</v>
+      <c r="F4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" t="s">
+        <v>129</v>
       </c>
       <c r="H4" t="s">
         <v>79</v>
@@ -941,16 +1529,14 @@
         <v>124</v>
       </c>
       <c r="E5" t="str">
-        <f>IF(LEFT(H5,1)="I","I",IF(LEFT(H5,1)="S","S",IF(LEFT(H5,1)="N","H",IF(LEFT(H5,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F5" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B5),",",H5," ",C5)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1402+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G5" t="str">
-        <f>CONCATENATE(D5,"_",E5,"_",B5,".png")</f>
-        <v>G_I_1402 6TH AVE NE.png</v>
+      <c r="F5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" t="s">
+        <v>130</v>
       </c>
       <c r="H5" t="s">
         <v>79</v>
@@ -970,16 +1556,14 @@
         <v>124</v>
       </c>
       <c r="E6" t="str">
-        <f>IF(LEFT(H6,1)="I","I",IF(LEFT(H6,1)="S","S",IF(LEFT(H6,1)="N","H",IF(LEFT(H6,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F6" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B6),",",H6," ",C6)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1501+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G6" t="str">
-        <f>CONCATENATE(D6,"_",E6,"_",B6,".png")</f>
-        <v>G_I_1501 NORTH RIDGE CT NE.png</v>
+      <c r="F6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G6" t="s">
+        <v>131</v>
       </c>
       <c r="H6" t="s">
         <v>79</v>
@@ -999,16 +1583,14 @@
         <v>124</v>
       </c>
       <c r="E7" t="str">
-        <f>IF(LEFT(H7,1)="I","I",IF(LEFT(H7,1)="S","S",IF(LEFT(H7,1)="N","H",IF(LEFT(H7,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F7" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B7),",",H7," ",C7)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1500+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G7" t="str">
-        <f>CONCATENATE(D7,"_",E7,"_",B7,".png")</f>
-        <v>G_I_1500 6TH AVE NE.png</v>
+      <c r="F7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" t="s">
+        <v>132</v>
       </c>
       <c r="H7" t="s">
         <v>79</v>
@@ -1028,16 +1610,14 @@
         <v>124</v>
       </c>
       <c r="E8" t="str">
-        <f>IF(LEFT(H8,1)="I","I",IF(LEFT(H8,1)="S","S",IF(LEFT(H8,1)="N","H",IF(LEFT(H8,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F8" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B8),",",H8," ",C8)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1502+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G8" t="str">
-        <f>CONCATENATE(D8,"_",E8,"_",B8,".png")</f>
-        <v>G_I_1502 NORTH RIDGE CT NE.png</v>
+      <c r="F8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" t="s">
+        <v>133</v>
       </c>
       <c r="H8" t="s">
         <v>79</v>
@@ -1057,16 +1637,14 @@
         <v>124</v>
       </c>
       <c r="E9" t="str">
-        <f>IF(LEFT(H9,1)="I","I",IF(LEFT(H9,1)="S","S",IF(LEFT(H9,1)="N","H",IF(LEFT(H9,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F9" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B9),",",H9," ",C9)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1503+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G9" t="str">
-        <f>CONCATENATE(D9,"_",E9,"_",B9,".png")</f>
-        <v>G_I_1503 NORTH RIDGE CT NE.png</v>
+      <c r="F9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G9" t="s">
+        <v>134</v>
       </c>
       <c r="H9" t="s">
         <v>79</v>
@@ -1086,16 +1664,14 @@
         <v>124</v>
       </c>
       <c r="E10" t="str">
-        <f>IF(LEFT(H10,1)="I","I",IF(LEFT(H10,1)="S","S",IF(LEFT(H10,1)="N","H",IF(LEFT(H10,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F10" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B10),",",H10," ",C10)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+14TH+ST+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G10" t="str">
-        <f>CONCATENATE(D10,"_",E10,"_",B10,".png")</f>
-        <v>G_I_502 14TH ST NE.png</v>
+      <c r="F10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G10" t="s">
+        <v>135</v>
       </c>
       <c r="H10" t="s">
         <v>79</v>
@@ -1115,16 +1691,14 @@
         <v>124</v>
       </c>
       <c r="E11" t="str">
-        <f>IF(LEFT(H11,1)="I","I",IF(LEFT(H11,1)="S","S",IF(LEFT(H11,1)="N","H",IF(LEFT(H11,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F11" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B11),",",H11," ",C11)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=504+14TH+ST+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G11" t="str">
-        <f>CONCATENATE(D11,"_",E11,"_",B11,".png")</f>
-        <v>G_I_504 14TH ST NE.png</v>
+      <c r="F11" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" t="s">
+        <v>136</v>
       </c>
       <c r="H11" t="s">
         <v>79</v>
@@ -1144,16 +1718,14 @@
         <v>124</v>
       </c>
       <c r="E12" t="str">
-        <f>IF(LEFT(H12,1)="I","I",IF(LEFT(H12,1)="S","S",IF(LEFT(H12,1)="N","H",IF(LEFT(H12,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F12" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B12),",",H12," ",C12)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=600+14TH+ST+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G12" t="str">
-        <f>CONCATENATE(D12,"_",E12,"_",B12,".png")</f>
-        <v>G_I_600 14TH ST NE.png</v>
+      <c r="F12" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" t="s">
+        <v>137</v>
       </c>
       <c r="H12" t="s">
         <v>79</v>
@@ -1173,16 +1745,14 @@
         <v>124</v>
       </c>
       <c r="E13" t="str">
-        <f>IF(LEFT(H13,1)="I","I",IF(LEFT(H13,1)="S","S",IF(LEFT(H13,1)="N","H",IF(LEFT(H13,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F13" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B13),",",H13," ",C13)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=602+14TH+ST+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G13" t="str">
-        <f>CONCATENATE(D13,"_",E13,"_",B13,".png")</f>
-        <v>G_I_602 14TH ST NE.png</v>
+      <c r="F13" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" t="s">
+        <v>138</v>
       </c>
       <c r="H13" t="s">
         <v>79</v>
@@ -1202,16 +1772,14 @@
         <v>124</v>
       </c>
       <c r="E14" t="str">
-        <f>IF(LEFT(H14,1)="I","I",IF(LEFT(H14,1)="S","S",IF(LEFT(H14,1)="N","H",IF(LEFT(H14,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F14" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B14),",",H14," ",C14)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1501+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G14" t="str">
-        <f>CONCATENATE(D14,"_",E14,"_",B14,".png")</f>
-        <v>G_I_1501 6TH AVE NE.png</v>
+      <c r="F14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" t="s">
+        <v>139</v>
       </c>
       <c r="H14" t="s">
         <v>79</v>
@@ -1231,16 +1799,14 @@
         <v>124</v>
       </c>
       <c r="E15" t="str">
-        <f>IF(LEFT(H15,1)="I","I",IF(LEFT(H15,1)="S","S",IF(LEFT(H15,1)="N","H",IF(LEFT(H15,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F15" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B15),",",H15," ",C15)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1502+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G15" t="str">
-        <f>CONCATENATE(D15,"_",E15,"_",B15,".png")</f>
-        <v>G_I_1502 6TH AVE NE.png</v>
+      <c r="F15" t="s">
+        <v>239</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
       </c>
       <c r="H15" t="s">
         <v>79</v>
@@ -1260,16 +1826,14 @@
         <v>124</v>
       </c>
       <c r="E16" t="str">
-        <f>IF(LEFT(H16,1)="I","I",IF(LEFT(H16,1)="S","S",IF(LEFT(H16,1)="N","H",IF(LEFT(H16,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F16" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B16),",",H16," ",C16)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1504+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G16" t="str">
-        <f>CONCATENATE(D16,"_",E16,"_",B16,".png")</f>
-        <v>G_I_1504 NORTH RIDGE CT NE.png</v>
+      <c r="F16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G16" t="s">
+        <v>141</v>
       </c>
       <c r="H16" t="s">
         <v>79</v>
@@ -1289,16 +1853,14 @@
         <v>124</v>
       </c>
       <c r="E17" t="str">
-        <f>IF(LEFT(H17,1)="I","I",IF(LEFT(H17,1)="S","S",IF(LEFT(H17,1)="N","H",IF(LEFT(H17,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F17" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B17),",",H17," ",C17)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1503+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G17" t="str">
-        <f>CONCATENATE(D17,"_",E17,"_",B17,".png")</f>
-        <v>G_I_1503 6TH AVE NE.png</v>
+      <c r="F17" t="s">
+        <v>241</v>
+      </c>
+      <c r="G17" t="s">
+        <v>142</v>
       </c>
       <c r="H17" t="s">
         <v>79</v>
@@ -1318,16 +1880,14 @@
         <v>124</v>
       </c>
       <c r="E18" t="str">
-        <f>IF(LEFT(H18,1)="I","I",IF(LEFT(H18,1)="S","S",IF(LEFT(H18,1)="N","H",IF(LEFT(H18,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F18" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B18),",",H18," ",C18)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1504+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G18" t="str">
-        <f>CONCATENATE(D18,"_",E18,"_",B18,".png")</f>
-        <v>G_I_1504 6TH AVE NE.png</v>
+      <c r="F18" t="s">
+        <v>242</v>
+      </c>
+      <c r="G18" t="s">
+        <v>143</v>
       </c>
       <c r="H18" t="s">
         <v>79</v>
@@ -1347,16 +1907,14 @@
         <v>124</v>
       </c>
       <c r="E19" t="str">
-        <f>IF(LEFT(H19,1)="I","I",IF(LEFT(H19,1)="S","S",IF(LEFT(H19,1)="N","H",IF(LEFT(H19,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F19" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B19),",",H19," ",C19)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1501+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G19" t="str">
-        <f>CONCATENATE(D19,"_",E19,"_",B19,".png")</f>
-        <v>G_I_1501 NORTH RIDGE CT NE.png</v>
+      <c r="F19" t="s">
+        <v>230</v>
+      </c>
+      <c r="G19" t="s">
+        <v>131</v>
       </c>
       <c r="H19" t="s">
         <v>79</v>
@@ -1376,16 +1934,14 @@
         <v>124</v>
       </c>
       <c r="E20" t="str">
-        <f>IF(LEFT(H20,1)="I","I",IF(LEFT(H20,1)="S","S",IF(LEFT(H20,1)="N","H",IF(LEFT(H20,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F20" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B20),",",H20," ",C20)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1506+NORTH+RIDGE+CT+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G20" t="str">
-        <f>CONCATENATE(D20,"_",E20,"_",B20,".png")</f>
-        <v>G_I_1506 NORTH RIDGE CT NE.png</v>
+      <c r="F20" t="s">
+        <v>243</v>
+      </c>
+      <c r="G20" t="s">
+        <v>144</v>
       </c>
       <c r="H20" t="s">
         <v>79</v>
@@ -1405,16 +1961,14 @@
         <v>124</v>
       </c>
       <c r="E21" t="str">
-        <f>IF(LEFT(H21,1)="I","I",IF(LEFT(H21,1)="S","S",IF(LEFT(H21,1)="N","H",IF(LEFT(H21,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F21" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B21),",",H21," ",C21)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1505+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G21" t="str">
-        <f>CONCATENATE(D21,"_",E21,"_",B21,".png")</f>
-        <v>G_I_1505 6TH AVE NE.png</v>
+      <c r="F21" t="s">
+        <v>244</v>
+      </c>
+      <c r="G21" t="s">
+        <v>145</v>
       </c>
       <c r="H21" t="s">
         <v>79</v>
@@ -1434,16 +1988,14 @@
         <v>124</v>
       </c>
       <c r="E22" t="str">
-        <f>IF(LEFT(H22,1)="I","I",IF(LEFT(H22,1)="S","S",IF(LEFT(H22,1)="N","H",IF(LEFT(H22,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F22" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B22),",",H22," ",C22)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1506+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G22" t="str">
-        <f>CONCATENATE(D22,"_",E22,"_",B22,".png")</f>
-        <v>G_I_1506 6TH AVE NE.png</v>
+      <c r="F22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G22" t="s">
+        <v>146</v>
       </c>
       <c r="H22" t="s">
         <v>79</v>
@@ -1463,16 +2015,14 @@
         <v>124</v>
       </c>
       <c r="E23" t="str">
-        <f>IF(LEFT(H23,1)="I","I",IF(LEFT(H23,1)="S","S",IF(LEFT(H23,1)="N","H",IF(LEFT(H23,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F23" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B23),",",H23," ",C23)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1803+8TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G23" t="str">
-        <f>CONCATENATE(D23,"_",E23,"_",B23,".png")</f>
-        <v>G_I_1803 8TH AVE NE.png</v>
+      <c r="F23" t="s">
+        <v>246</v>
+      </c>
+      <c r="G23" t="s">
+        <v>147</v>
       </c>
       <c r="H23" t="s">
         <v>79</v>
@@ -1492,16 +2042,14 @@
         <v>124</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(LEFT(H24,1)="I","I",IF(LEFT(H24,1)="S","S",IF(LEFT(H24,1)="N","H",IF(LEFT(H24,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F24" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B24),",",H24," ",C24)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=2089+KENTUCKY+AVE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G24" t="str">
-        <f>CONCATENATE(D24,"_",E24,"_",B24,".png")</f>
-        <v>G_I_2089 KENTUCKY AVE.png</v>
+      <c r="F24" t="s">
+        <v>247</v>
+      </c>
+      <c r="G24" t="s">
+        <v>148</v>
       </c>
       <c r="H24" t="s">
         <v>79</v>
@@ -1521,16 +2069,14 @@
         <v>124</v>
       </c>
       <c r="E25" t="str">
-        <f>IF(LEFT(H25,1)="I","I",IF(LEFT(H25,1)="S","S",IF(LEFT(H25,1)="N","H",IF(LEFT(H25,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F25" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B25),",",H25," ",C25)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1508+6TH+AVE+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G25" t="str">
-        <f>CONCATENATE(D25,"_",E25,"_",B25,".png")</f>
-        <v>G_I_1508 6TH AVE NE.png</v>
+      <c r="F25" t="s">
+        <v>248</v>
+      </c>
+      <c r="G25" t="s">
+        <v>149</v>
       </c>
       <c r="H25" t="s">
         <v>79</v>
@@ -1550,16 +2096,14 @@
         <v>124</v>
       </c>
       <c r="E26" t="str">
-        <f>IF(LEFT(H26,1)="I","I",IF(LEFT(H26,1)="S","S",IF(LEFT(H26,1)="N","H",IF(LEFT(H26,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
-      <c r="F26" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B26),",",H26," ",C26)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+16TH+ST+NE,INDEPENDENCE+IOWA</v>
-      </c>
-      <c r="G26" t="str">
-        <f>CONCATENATE(D26,"_",E26,"_",B26,".png")</f>
-        <v>G_I_502 16TH ST NE.png</v>
+      <c r="F26" t="s">
+        <v>249</v>
+      </c>
+      <c r="G26" t="s">
+        <v>150</v>
       </c>
       <c r="H26" t="s">
         <v>79</v>
@@ -1579,16 +2123,14 @@
         <v>124</v>
       </c>
       <c r="E27" t="str">
-        <f>IF(LEFT(H27,1)="I","I",IF(LEFT(H27,1)="S","S",IF(LEFT(H27,1)="N","H",IF(LEFT(H27,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F27" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B27),",",H27," ",C27)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=116+N+CHESTNUT+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G27" t="str">
-        <f>CONCATENATE(D27,"_",E27,"_",B27,".png")</f>
-        <v>G_H_116 N CHESTNUT ST.png</v>
+      <c r="F27" t="s">
+        <v>250</v>
+      </c>
+      <c r="G27" t="s">
+        <v>151</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1608,16 +2150,14 @@
         <v>124</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(LEFT(H28,1)="I","I",IF(LEFT(H28,1)="S","S",IF(LEFT(H28,1)="N","H",IF(LEFT(H28,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F28" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B28),",",H28," ",C28)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=12+E+COURT+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G28" t="str">
-        <f>CONCATENATE(D28,"_",E28,"_",B28,".png")</f>
-        <v>G_H_12 E COURT ST.png</v>
+      <c r="F28" t="s">
+        <v>251</v>
+      </c>
+      <c r="G28" t="s">
+        <v>152</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -1637,16 +2177,14 @@
         <v>124</v>
       </c>
       <c r="E29" t="str">
-        <f>IF(LEFT(H29,1)="I","I",IF(LEFT(H29,1)="S","S",IF(LEFT(H29,1)="N","H",IF(LEFT(H29,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F29" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B29),",",H29," ",C29)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=311+W+MAIN+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G29" t="str">
-        <f>CONCATENATE(D29,"_",E29,"_",B29,".png")</f>
-        <v>G_H_311 W MAIN ST.png</v>
+      <c r="F29" t="s">
+        <v>252</v>
+      </c>
+      <c r="G29" t="s">
+        <v>153</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -1666,16 +2204,14 @@
         <v>124</v>
       </c>
       <c r="E30" t="str">
-        <f>IF(LEFT(H30,1)="I","I",IF(LEFT(H30,1)="S","S",IF(LEFT(H30,1)="N","H",IF(LEFT(H30,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F30" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B30),",",H30," ",C30)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=102+E+MAIN+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G30" t="str">
-        <f>CONCATENATE(D30,"_",E30,"_",B30,".png")</f>
-        <v>G_H_102 E MAIN ST.png</v>
+      <c r="F30" t="s">
+        <v>253</v>
+      </c>
+      <c r="G30" t="s">
+        <v>154</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -1695,16 +2231,14 @@
         <v>124</v>
       </c>
       <c r="E31" t="str">
-        <f>IF(LEFT(H31,1)="I","I",IF(LEFT(H31,1)="S","S",IF(LEFT(H31,1)="N","H",IF(LEFT(H31,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F31" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B31),",",H31," ",C31)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=508+N+LINN+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G31" t="str">
-        <f>CONCATENATE(D31,"_",E31,"_",B31,".png")</f>
-        <v>G_H_508 N LINN AVE.png</v>
+      <c r="F31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G31" t="s">
+        <v>155</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -1724,16 +2258,14 @@
         <v>124</v>
       </c>
       <c r="E32" t="str">
-        <f>IF(LEFT(H32,1)="I","I",IF(LEFT(H32,1)="S","S",IF(LEFT(H32,1)="N","H",IF(LEFT(H32,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F32" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B32),",",H32," ",C32)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=9+W+GARDNER+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G32" t="str">
-        <f>CONCATENATE(D32,"_",E32,"_",B32,".png")</f>
-        <v>G_H_9 W GARDNER ST.png</v>
+      <c r="F32" t="s">
+        <v>255</v>
+      </c>
+      <c r="G32" t="s">
+        <v>156</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -1753,16 +2285,14 @@
         <v>124</v>
       </c>
       <c r="E33" t="str">
-        <f>IF(LEFT(H33,1)="I","I",IF(LEFT(H33,1)="S","S",IF(LEFT(H33,1)="N","H",IF(LEFT(H33,1)="G","D"))))</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="F33" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B33),",",H33," ",C33)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=7+W+COURT+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G33" t="str">
-        <f>CONCATENATE(D33,"_",E33,"_",B33,".png")</f>
-        <v>G_H_7 W COURT ST.png</v>
+      <c r="F33" t="s">
+        <v>256</v>
+      </c>
+      <c r="G33" t="s">
+        <v>157</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
@@ -1782,16 +2312,14 @@
         <v>124</v>
       </c>
       <c r="E34" t="str">
-        <f>IF(LEFT(H34,1)="I","I",IF(LEFT(H34,1)="S","S",IF(LEFT(H34,1)="N","H",IF(LEFT(H34,1)="G","D"))))</f>
+        <f t="shared" ref="E34:E65" si="1">IF(LEFT(H34,1)="I","I",IF(LEFT(H34,1)="S","S",IF(LEFT(H34,1)="N","H",IF(LEFT(H34,1)="G","D"))))</f>
         <v>H</v>
       </c>
-      <c r="F34" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B34),",",H34," ",C34)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=213+N+WALNUT+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G34" t="str">
-        <f>CONCATENATE(D34,"_",E34,"_",B34,".png")</f>
-        <v>G_H_213 N WALNUT AVE.png</v>
+      <c r="F34" t="s">
+        <v>257</v>
+      </c>
+      <c r="G34" t="s">
+        <v>158</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -1811,16 +2339,14 @@
         <v>124</v>
       </c>
       <c r="E35" t="str">
-        <f>IF(LEFT(H35,1)="I","I",IF(LEFT(H35,1)="S","S",IF(LEFT(H35,1)="N","H",IF(LEFT(H35,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F35" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B35),",",H35," ",C35)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=22+N+LINN+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G35" t="str">
-        <f>CONCATENATE(D35,"_",E35,"_",B35,".png")</f>
-        <v>G_H_22 N LINN AVE.png</v>
+      <c r="F35" t="s">
+        <v>258</v>
+      </c>
+      <c r="G35" t="s">
+        <v>159</v>
       </c>
       <c r="H35" t="s">
         <v>4</v>
@@ -1840,16 +2366,14 @@
         <v>124</v>
       </c>
       <c r="E36" t="str">
-        <f>IF(LEFT(H36,1)="I","I",IF(LEFT(H36,1)="S","S",IF(LEFT(H36,1)="N","H",IF(LEFT(H36,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F36" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B36),",",H36," ",C36)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=316+N+WALNUT+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G36" t="str">
-        <f>CONCATENATE(D36,"_",E36,"_",B36,".png")</f>
-        <v>G_H_316 N WALNUT AVE.png</v>
+      <c r="F36" t="s">
+        <v>259</v>
+      </c>
+      <c r="G36" t="s">
+        <v>160</v>
       </c>
       <c r="H36" t="s">
         <v>4</v>
@@ -1869,16 +2393,14 @@
         <v>124</v>
       </c>
       <c r="E37" t="str">
-        <f>IF(LEFT(H37,1)="I","I",IF(LEFT(H37,1)="S","S",IF(LEFT(H37,1)="N","H",IF(LEFT(H37,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F37" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B37),",",H37," ",C37)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=14+E+WASHINGTON+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G37" t="str">
-        <f>CONCATENATE(D37,"_",E37,"_",B37,".png")</f>
-        <v>G_H_14 E WASHINGTON ST.png</v>
+      <c r="F37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G37" t="s">
+        <v>161</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
@@ -1898,16 +2420,14 @@
         <v>124</v>
       </c>
       <c r="E38" t="str">
-        <f>IF(LEFT(H38,1)="I","I",IF(LEFT(H38,1)="S","S",IF(LEFT(H38,1)="N","H",IF(LEFT(H38,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F38" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B38),",",H38," ",C38)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=311+N+LOCUST+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G38" t="str">
-        <f>CONCATENATE(D38,"_",E38,"_",B38,".png")</f>
-        <v>G_H_311 N LOCUST AVE.png</v>
+      <c r="F38" t="s">
+        <v>261</v>
+      </c>
+      <c r="G38" t="s">
+        <v>162</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
@@ -1927,16 +2447,14 @@
         <v>124</v>
       </c>
       <c r="E39" t="str">
-        <f>IF(LEFT(H39,1)="I","I",IF(LEFT(H39,1)="S","S",IF(LEFT(H39,1)="N","H",IF(LEFT(H39,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F39" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B39),",",H39," ",C39)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=101+N+LOCUST+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G39" t="str">
-        <f>CONCATENATE(D39,"_",E39,"_",B39,".png")</f>
-        <v>G_H_101 N LOCUST AVE.png</v>
+      <c r="F39" t="s">
+        <v>262</v>
+      </c>
+      <c r="G39" t="s">
+        <v>163</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
@@ -1956,16 +2474,14 @@
         <v>124</v>
       </c>
       <c r="E40" t="str">
-        <f>IF(LEFT(H40,1)="I","I",IF(LEFT(H40,1)="S","S",IF(LEFT(H40,1)="N","H",IF(LEFT(H40,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F40" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B40),",",H40," ",C40)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=615+N+LINN+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G40" t="str">
-        <f>CONCATENATE(D40,"_",E40,"_",B40,".png")</f>
-        <v>G_H_615 N LINN AVE.png</v>
+      <c r="F40" t="s">
+        <v>263</v>
+      </c>
+      <c r="G40" t="s">
+        <v>164</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -1985,16 +2501,14 @@
         <v>124</v>
       </c>
       <c r="E41" t="str">
-        <f>IF(LEFT(H41,1)="I","I",IF(LEFT(H41,1)="S","S",IF(LEFT(H41,1)="N","H",IF(LEFT(H41,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F41" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B41),",",H41," ",C41)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=206+N+FOLEY+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G41" t="str">
-        <f>CONCATENATE(D41,"_",E41,"_",B41,".png")</f>
-        <v>G_H_206 N FOLEY AVE.png</v>
+      <c r="F41" t="s">
+        <v>264</v>
+      </c>
+      <c r="G41" t="s">
+        <v>165</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -2014,16 +2528,14 @@
         <v>124</v>
       </c>
       <c r="E42" t="str">
-        <f>IF(LEFT(H42,1)="I","I",IF(LEFT(H42,1)="S","S",IF(LEFT(H42,1)="N","H",IF(LEFT(H42,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F42" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B42),",",H42," ",C42)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=214+E+WASHINGTON+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G42" t="str">
-        <f>CONCATENATE(D42,"_",E42,"_",B42,".png")</f>
-        <v>G_H_214 E WASHINGTON ST.png</v>
+      <c r="F42" t="s">
+        <v>265</v>
+      </c>
+      <c r="G42" t="s">
+        <v>166</v>
       </c>
       <c r="H42" t="s">
         <v>4</v>
@@ -2043,16 +2555,14 @@
         <v>124</v>
       </c>
       <c r="E43" t="str">
-        <f>IF(LEFT(H43,1)="I","I",IF(LEFT(H43,1)="S","S",IF(LEFT(H43,1)="N","H",IF(LEFT(H43,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F43" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B43),",",H43," ",C43)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=206+N+LINN+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G43" t="str">
-        <f>CONCATENATE(D43,"_",E43,"_",B43,".png")</f>
-        <v>G_H_206 N LINN AVE.png</v>
+      <c r="F43" t="s">
+        <v>266</v>
+      </c>
+      <c r="G43" t="s">
+        <v>167</v>
       </c>
       <c r="H43" t="s">
         <v>4</v>
@@ -2072,16 +2582,14 @@
         <v>124</v>
       </c>
       <c r="E44" t="str">
-        <f>IF(LEFT(H44,1)="I","I",IF(LEFT(H44,1)="S","S",IF(LEFT(H44,1)="N","H",IF(LEFT(H44,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F44" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B44),",",H44," ",C44)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=102+N+LINN+AVE,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G44" t="str">
-        <f>CONCATENATE(D44,"_",E44,"_",B44,".png")</f>
-        <v>G_H_102 N LINN AVE.png</v>
+      <c r="F44" t="s">
+        <v>267</v>
+      </c>
+      <c r="G44" t="s">
+        <v>168</v>
       </c>
       <c r="H44" t="s">
         <v>4</v>
@@ -2101,16 +2609,14 @@
         <v>124</v>
       </c>
       <c r="E45" t="str">
-        <f>IF(LEFT(H45,1)="I","I",IF(LEFT(H45,1)="S","S",IF(LEFT(H45,1)="N","H",IF(LEFT(H45,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F45" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B45),",",H45," ",C45)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=313+E+MILWAUKEE+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G45" t="str">
-        <f>CONCATENATE(D45,"_",E45,"_",B45,".png")</f>
-        <v>G_H_313 E MILWAUKEE ST.png</v>
+      <c r="F45" t="s">
+        <v>268</v>
+      </c>
+      <c r="G45" t="s">
+        <v>169</v>
       </c>
       <c r="H45" t="s">
         <v>4</v>
@@ -2130,16 +2636,14 @@
         <v>124</v>
       </c>
       <c r="E46" t="str">
-        <f>IF(LEFT(H46,1)="I","I",IF(LEFT(H46,1)="S","S",IF(LEFT(H46,1)="N","H",IF(LEFT(H46,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F46" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B46),",",H46," ",C46)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=4+E+HALE+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G46" t="str">
-        <f>CONCATENATE(D46,"_",E46,"_",B46,".png")</f>
-        <v>G_H_4 E HALE ST.png</v>
+      <c r="F46" t="s">
+        <v>269</v>
+      </c>
+      <c r="G46" t="s">
+        <v>170</v>
       </c>
       <c r="H46" t="s">
         <v>4</v>
@@ -2159,16 +2663,14 @@
         <v>124</v>
       </c>
       <c r="E47" t="str">
-        <f>IF(LEFT(H47,1)="I","I",IF(LEFT(H47,1)="S","S",IF(LEFT(H47,1)="N","H",IF(LEFT(H47,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F47" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B47),",",H47," ",C47)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=104+E+MAIN+ST,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G47" t="str">
-        <f>CONCATENATE(D47,"_",E47,"_",B47,".png")</f>
-        <v>G_H_104 E MAIN ST.png</v>
+      <c r="F47" t="s">
+        <v>270</v>
+      </c>
+      <c r="G47" t="s">
+        <v>171</v>
       </c>
       <c r="H47" t="s">
         <v>4</v>
@@ -2188,16 +2690,14 @@
         <v>124</v>
       </c>
       <c r="E48" t="str">
-        <f>IF(LEFT(H48,1)="I","I",IF(LEFT(H48,1)="S","S",IF(LEFT(H48,1)="N","H",IF(LEFT(H48,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F48" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B48),",",H48," ",C48)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=602+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G48" t="str">
-        <f>CONCATENATE(D48,"_",E48,"_",B48,".png")</f>
-        <v>G_H_602 HOMESTEAD CIR.png</v>
+      <c r="F48" t="s">
+        <v>271</v>
+      </c>
+      <c r="G48" t="s">
+        <v>172</v>
       </c>
       <c r="H48" t="s">
         <v>4</v>
@@ -2217,16 +2717,14 @@
         <v>124</v>
       </c>
       <c r="E49" t="str">
-        <f>IF(LEFT(H49,1)="I","I",IF(LEFT(H49,1)="S","S",IF(LEFT(H49,1)="N","H",IF(LEFT(H49,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F49" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B49),",",H49," ",C49)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=607+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G49" t="str">
-        <f>CONCATENATE(D49,"_",E49,"_",B49,".png")</f>
-        <v>G_H_607 HOMESTEAD CIR.png</v>
+      <c r="F49" t="s">
+        <v>272</v>
+      </c>
+      <c r="G49" t="s">
+        <v>173</v>
       </c>
       <c r="H49" t="s">
         <v>4</v>
@@ -2246,16 +2744,14 @@
         <v>124</v>
       </c>
       <c r="E50" t="str">
-        <f>IF(LEFT(H50,1)="I","I",IF(LEFT(H50,1)="S","S",IF(LEFT(H50,1)="N","H",IF(LEFT(H50,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F50" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B50),",",H50," ",C50)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=616+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G50" t="str">
-        <f>CONCATENATE(D50,"_",E50,"_",B50,".png")</f>
-        <v>G_H_616 HOMESTEAD CIR.png</v>
+      <c r="F50" t="s">
+        <v>273</v>
+      </c>
+      <c r="G50" t="s">
+        <v>174</v>
       </c>
       <c r="H50" t="s">
         <v>4</v>
@@ -2275,16 +2771,14 @@
         <v>124</v>
       </c>
       <c r="E51" t="str">
-        <f>IF(LEFT(H51,1)="I","I",IF(LEFT(H51,1)="S","S",IF(LEFT(H51,1)="N","H",IF(LEFT(H51,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="F51" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B51),",",H51," ",C51)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=601+HOMESTEAD+CIR,NEW+HAMPTON+IOWA</v>
-      </c>
-      <c r="G51" t="str">
-        <f>CONCATENATE(D51,"_",E51,"_",B51,".png")</f>
-        <v>G_H_601 HOMESTEAD CIR.png</v>
+      <c r="F51" t="s">
+        <v>274</v>
+      </c>
+      <c r="G51" t="s">
+        <v>175</v>
       </c>
       <c r="H51" t="s">
         <v>4</v>
@@ -2304,16 +2798,14 @@
         <v>124</v>
       </c>
       <c r="E52" t="str">
-        <f>IF(LEFT(H52,1)="I","I",IF(LEFT(H52,1)="S","S",IF(LEFT(H52,1)="N","H",IF(LEFT(H52,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F52" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B52),",",H52," ",C52)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=701+BENTON+CIR,SLATER+IOWA</v>
-      </c>
-      <c r="G52" t="str">
-        <f>CONCATENATE(D52,"_",E52,"_",B52,".png")</f>
-        <v>G_S_ 701 BENTON CIR .png</v>
+      <c r="F52" t="s">
+        <v>275</v>
+      </c>
+      <c r="G52" t="s">
+        <v>176</v>
       </c>
       <c r="H52" t="s">
         <v>30</v>
@@ -2333,16 +2825,14 @@
         <v>124</v>
       </c>
       <c r="E53" t="str">
-        <f>IF(LEFT(H53,1)="I","I",IF(LEFT(H53,1)="S","S",IF(LEFT(H53,1)="N","H",IF(LEFT(H53,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F53" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B53),",",H53," ",C53)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=637+GREENE+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G53" t="str">
-        <f>CONCATENATE(D53,"_",E53,"_",B53,".png")</f>
-        <v>G_S_ 637 GREENE ST .png</v>
+      <c r="F53" t="s">
+        <v>276</v>
+      </c>
+      <c r="G53" t="s">
+        <v>177</v>
       </c>
       <c r="H53" t="s">
         <v>30</v>
@@ -2362,16 +2852,14 @@
         <v>124</v>
       </c>
       <c r="E54" t="str">
-        <f>IF(LEFT(H54,1)="I","I",IF(LEFT(H54,1)="S","S",IF(LEFT(H54,1)="N","H",IF(LEFT(H54,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F54" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B54),",",H54," ",C54)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=705+TAMA+CIR,SLATER+IOWA</v>
-      </c>
-      <c r="G54" t="str">
-        <f>CONCATENATE(D54,"_",E54,"_",B54,".png")</f>
-        <v>G_S_ 705 TAMA CIR .png</v>
+      <c r="F54" t="s">
+        <v>277</v>
+      </c>
+      <c r="G54" t="s">
+        <v>178</v>
       </c>
       <c r="H54" t="s">
         <v>30</v>
@@ -2391,16 +2879,14 @@
         <v>124</v>
       </c>
       <c r="E55" t="str">
-        <f>IF(LEFT(H55,1)="I","I",IF(LEFT(H55,1)="S","S",IF(LEFT(H55,1)="N","H",IF(LEFT(H55,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F55" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B55),",",H55," ",C55)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=608+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G55" t="str">
-        <f>CONCATENATE(D55,"_",E55,"_",B55,".png")</f>
-        <v>G_S_ 608 8TH AVE .png</v>
+      <c r="F55" t="s">
+        <v>278</v>
+      </c>
+      <c r="G55" t="s">
+        <v>179</v>
       </c>
       <c r="H55" t="s">
         <v>30</v>
@@ -2420,16 +2906,14 @@
         <v>124</v>
       </c>
       <c r="E56" t="str">
-        <f>IF(LEFT(H56,1)="I","I",IF(LEFT(H56,1)="S","S",IF(LEFT(H56,1)="N","H",IF(LEFT(H56,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F56" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B56),",",H56," ",C56)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=604+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G56" t="str">
-        <f>CONCATENATE(D56,"_",E56,"_",B56,".png")</f>
-        <v>G_S_ 604 8TH AVE .png</v>
+      <c r="F56" t="s">
+        <v>279</v>
+      </c>
+      <c r="G56" t="s">
+        <v>180</v>
       </c>
       <c r="H56" t="s">
         <v>30</v>
@@ -2449,16 +2933,14 @@
         <v>124</v>
       </c>
       <c r="E57" t="str">
-        <f>IF(LEFT(H57,1)="I","I",IF(LEFT(H57,1)="S","S",IF(LEFT(H57,1)="N","H",IF(LEFT(H57,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F57" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B57),",",H57," ",C57)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=202+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G57" t="str">
-        <f>CONCATENATE(D57,"_",E57,"_",B57,".png")</f>
-        <v>G_S_ 202 8TH AVE .png</v>
+      <c r="F57" t="s">
+        <v>280</v>
+      </c>
+      <c r="G57" t="s">
+        <v>181</v>
       </c>
       <c r="H57" t="s">
         <v>30</v>
@@ -2478,16 +2960,14 @@
         <v>124</v>
       </c>
       <c r="E58" t="str">
-        <f>IF(LEFT(H58,1)="I","I",IF(LEFT(H58,1)="S","S",IF(LEFT(H58,1)="N","H",IF(LEFT(H58,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F58" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B58),",",H58," ",C58)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=104+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G58" t="str">
-        <f>CONCATENATE(D58,"_",E58,"_",B58,".png")</f>
-        <v>G_S_ 104 8TH AVE .png</v>
+      <c r="F58" t="s">
+        <v>281</v>
+      </c>
+      <c r="G58" t="s">
+        <v>182</v>
       </c>
       <c r="H58" t="s">
         <v>30</v>
@@ -2507,16 +2987,14 @@
         <v>124</v>
       </c>
       <c r="E59" t="str">
-        <f>IF(LEFT(H59,1)="I","I",IF(LEFT(H59,1)="S","S",IF(LEFT(H59,1)="N","H",IF(LEFT(H59,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F59" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B59),",",H59," ",C59)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=706+MARSHALL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G59" t="str">
-        <f>CONCATENATE(D59,"_",E59,"_",B59,".png")</f>
-        <v>G_S_ 706 MARSHALL ST .png</v>
+      <c r="F59" t="s">
+        <v>282</v>
+      </c>
+      <c r="G59" t="s">
+        <v>183</v>
       </c>
       <c r="H59" t="s">
         <v>30</v>
@@ -2536,16 +3014,14 @@
         <v>124</v>
       </c>
       <c r="E60" t="str">
-        <f>IF(LEFT(H60,1)="I","I",IF(LEFT(H60,1)="S","S",IF(LEFT(H60,1)="N","H",IF(LEFT(H60,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F60" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B60),",",H60," ",C60)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=900+FOUR+MILE+DR,SLATER+IOWA</v>
-      </c>
-      <c r="G60" t="str">
-        <f>CONCATENATE(D60,"_",E60,"_",B60,".png")</f>
-        <v>G_S_ 900 FOUR MILE DR .png</v>
+      <c r="F60" t="s">
+        <v>283</v>
+      </c>
+      <c r="G60" t="s">
+        <v>184</v>
       </c>
       <c r="H60" t="s">
         <v>30</v>
@@ -2565,16 +3041,14 @@
         <v>124</v>
       </c>
       <c r="E61" t="str">
-        <f>IF(LEFT(H61,1)="I","I",IF(LEFT(H61,1)="S","S",IF(LEFT(H61,1)="N","H",IF(LEFT(H61,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F61" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B61),",",H61," ",C61)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=638+GREENE+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G61" t="str">
-        <f>CONCATENATE(D61,"_",E61,"_",B61,".png")</f>
-        <v>G_S_ 638 GREENE ST .png</v>
+      <c r="F61" t="s">
+        <v>284</v>
+      </c>
+      <c r="G61" t="s">
+        <v>185</v>
       </c>
       <c r="H61" t="s">
         <v>30</v>
@@ -2594,16 +3068,14 @@
         <v>124</v>
       </c>
       <c r="E62" t="str">
-        <f>IF(LEFT(H62,1)="I","I",IF(LEFT(H62,1)="S","S",IF(LEFT(H62,1)="N","H",IF(LEFT(H62,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F62" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B62),",",H62," ",C62)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=700+TAMA+CIR,SLATER+IOWA</v>
-      </c>
-      <c r="G62" t="str">
-        <f>CONCATENATE(D62,"_",E62,"_",B62,".png")</f>
-        <v>G_S_ 700 TAMA CIR .png</v>
+      <c r="F62" t="s">
+        <v>285</v>
+      </c>
+      <c r="G62" t="s">
+        <v>186</v>
       </c>
       <c r="H62" t="s">
         <v>30</v>
@@ -2623,16 +3095,14 @@
         <v>124</v>
       </c>
       <c r="E63" t="str">
-        <f>IF(LEFT(H63,1)="I","I",IF(LEFT(H63,1)="S","S",IF(LEFT(H63,1)="N","H",IF(LEFT(H63,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F63" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B63),",",H63," ",C63)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=705+BENTON+CIR,SLATER+IOWA</v>
-      </c>
-      <c r="G63" t="str">
-        <f>CONCATENATE(D63,"_",E63,"_",B63,".png")</f>
-        <v>G_S_ 705 BENTON CIR .png</v>
+      <c r="F63" t="s">
+        <v>286</v>
+      </c>
+      <c r="G63" t="s">
+        <v>187</v>
       </c>
       <c r="H63" t="s">
         <v>30</v>
@@ -2652,16 +3122,14 @@
         <v>124</v>
       </c>
       <c r="E64" t="str">
-        <f>IF(LEFT(H64,1)="I","I",IF(LEFT(H64,1)="S","S",IF(LEFT(H64,1)="N","H",IF(LEFT(H64,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F64" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B64),",",H64," ",C64)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=700+BENTON+CIR,SLATER+IOWA</v>
-      </c>
-      <c r="G64" t="str">
-        <f>CONCATENATE(D64,"_",E64,"_",B64,".png")</f>
-        <v>G_S_ 700 BENTON CIR .png</v>
+      <c r="F64" t="s">
+        <v>287</v>
+      </c>
+      <c r="G64" t="s">
+        <v>188</v>
       </c>
       <c r="H64" t="s">
         <v>30</v>
@@ -2681,16 +3149,14 @@
         <v>124</v>
       </c>
       <c r="E65" t="str">
-        <f>IF(LEFT(H65,1)="I","I",IF(LEFT(H65,1)="S","S",IF(LEFT(H65,1)="N","H",IF(LEFT(H65,1)="G","D"))))</f>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="F65" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B65),",",H65," ",C65)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=610+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G65" t="str">
-        <f>CONCATENATE(D65,"_",E65,"_",B65,".png")</f>
-        <v>G_S_ 610 8TH AVE .png</v>
+      <c r="F65" t="s">
+        <v>288</v>
+      </c>
+      <c r="G65" t="s">
+        <v>189</v>
       </c>
       <c r="H65" t="s">
         <v>30</v>
@@ -2710,16 +3176,14 @@
         <v>124</v>
       </c>
       <c r="E66" t="str">
-        <f>IF(LEFT(H66,1)="I","I",IF(LEFT(H66,1)="S","S",IF(LEFT(H66,1)="N","H",IF(LEFT(H66,1)="G","D"))))</f>
+        <f t="shared" ref="E66:E101" si="2">IF(LEFT(H66,1)="I","I",IF(LEFT(H66,1)="S","S",IF(LEFT(H66,1)="N","H",IF(LEFT(H66,1)="G","D"))))</f>
         <v>S</v>
       </c>
-      <c r="F66" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B66),",",H66," ",C66)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=204+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G66" t="str">
-        <f>CONCATENATE(D66,"_",E66,"_",B66,".png")</f>
-        <v>G_S_ 204 8TH AVE .png</v>
+      <c r="F66" t="s">
+        <v>289</v>
+      </c>
+      <c r="G66" t="s">
+        <v>190</v>
       </c>
       <c r="H66" t="s">
         <v>30</v>
@@ -2739,16 +3203,14 @@
         <v>124</v>
       </c>
       <c r="E67" t="str">
-        <f>IF(LEFT(H67,1)="I","I",IF(LEFT(H67,1)="S","S",IF(LEFT(H67,1)="N","H",IF(LEFT(H67,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F67" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B67),",",H67," ",C67)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=614+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G67" t="str">
-        <f>CONCATENATE(D67,"_",E67,"_",B67,".png")</f>
-        <v>G_S_ 614 8TH AVE .png</v>
+      <c r="F67" t="s">
+        <v>290</v>
+      </c>
+      <c r="G67" t="s">
+        <v>191</v>
       </c>
       <c r="H67" t="s">
         <v>30</v>
@@ -2768,16 +3230,14 @@
         <v>124</v>
       </c>
       <c r="E68" t="str">
-        <f>IF(LEFT(H68,1)="I","I",IF(LEFT(H68,1)="S","S",IF(LEFT(H68,1)="N","H",IF(LEFT(H68,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F68" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B68),",",H68," ",C68)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=708+MARSHALL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G68" t="str">
-        <f>CONCATENATE(D68,"_",E68,"_",B68,".png")</f>
-        <v>G_S_ 708 MARSHALL ST .png</v>
+      <c r="F68" t="s">
+        <v>291</v>
+      </c>
+      <c r="G68" t="s">
+        <v>192</v>
       </c>
       <c r="H68" t="s">
         <v>30</v>
@@ -2797,16 +3257,14 @@
         <v>124</v>
       </c>
       <c r="E69" t="str">
-        <f>IF(LEFT(H69,1)="I","I",IF(LEFT(H69,1)="S","S",IF(LEFT(H69,1)="N","H",IF(LEFT(H69,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F69" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B69),",",H69," ",C69)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=101+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G69" t="str">
-        <f>CONCATENATE(D69,"_",E69,"_",B69,".png")</f>
-        <v>G_S_ 101 8TH AVE .png</v>
+      <c r="F69" t="s">
+        <v>292</v>
+      </c>
+      <c r="G69" t="s">
+        <v>193</v>
       </c>
       <c r="H69" t="s">
         <v>30</v>
@@ -2826,16 +3284,14 @@
         <v>124</v>
       </c>
       <c r="E70" t="str">
-        <f>IF(LEFT(H70,1)="I","I",IF(LEFT(H70,1)="S","S",IF(LEFT(H70,1)="N","H",IF(LEFT(H70,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F70" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B70),",",H70," ",C70)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=100+8TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G70" t="str">
-        <f>CONCATENATE(D70,"_",E70,"_",B70,".png")</f>
-        <v>G_S_ 100 8TH AVE .png</v>
+      <c r="F70" t="s">
+        <v>293</v>
+      </c>
+      <c r="G70" t="s">
+        <v>194</v>
       </c>
       <c r="H70" t="s">
         <v>30</v>
@@ -2855,16 +3311,14 @@
         <v>124</v>
       </c>
       <c r="E71" t="str">
-        <f>IF(LEFT(H71,1)="I","I",IF(LEFT(H71,1)="S","S",IF(LEFT(H71,1)="N","H",IF(LEFT(H71,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F71" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B71),",",H71," ",C71)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=305+9TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G71" t="str">
-        <f>CONCATENATE(D71,"_",E71,"_",B71,".png")</f>
-        <v>G_S_ 305 9TH AVE .png</v>
+      <c r="F71" t="s">
+        <v>294</v>
+      </c>
+      <c r="G71" t="s">
+        <v>195</v>
       </c>
       <c r="H71" t="s">
         <v>30</v>
@@ -2884,16 +3338,14 @@
         <v>124</v>
       </c>
       <c r="E72" t="str">
-        <f>IF(LEFT(H72,1)="I","I",IF(LEFT(H72,1)="S","S",IF(LEFT(H72,1)="N","H",IF(LEFT(H72,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F72" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B72),",",H72," ",C72)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=804+S+CARROLL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G72" t="str">
-        <f>CONCATENATE(D72,"_",E72,"_",B72,".png")</f>
-        <v>G_S_ 804 S CARROLL ST .png</v>
+      <c r="F72" t="s">
+        <v>295</v>
+      </c>
+      <c r="G72" t="s">
+        <v>196</v>
       </c>
       <c r="H72" t="s">
         <v>30</v>
@@ -2913,16 +3365,14 @@
         <v>124</v>
       </c>
       <c r="E73" t="str">
-        <f>IF(LEFT(H73,1)="I","I",IF(LEFT(H73,1)="S","S",IF(LEFT(H73,1)="N","H",IF(LEFT(H73,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F73" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B73),",",H73," ",C73)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=605+MARSHALL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G73" t="str">
-        <f>CONCATENATE(D73,"_",E73,"_",B73,".png")</f>
-        <v>G_S_ 605 MARSHALL ST .png</v>
+      <c r="F73" t="s">
+        <v>296</v>
+      </c>
+      <c r="G73" t="s">
+        <v>197</v>
       </c>
       <c r="H73" t="s">
         <v>30</v>
@@ -2942,16 +3392,14 @@
         <v>124</v>
       </c>
       <c r="E74" t="str">
-        <f>IF(LEFT(H74,1)="I","I",IF(LEFT(H74,1)="S","S",IF(LEFT(H74,1)="N","H",IF(LEFT(H74,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F74" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B74),",",H74," ",C74)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=807+S+CARROLL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G74" t="str">
-        <f>CONCATENATE(D74,"_",E74,"_",B74,".png")</f>
-        <v>G_S_ 807 S CARROLL ST .png</v>
+      <c r="F74" t="s">
+        <v>297</v>
+      </c>
+      <c r="G74" t="s">
+        <v>198</v>
       </c>
       <c r="H74" t="s">
         <v>30</v>
@@ -2971,16 +3419,14 @@
         <v>124</v>
       </c>
       <c r="E75" t="str">
-        <f>IF(LEFT(H75,1)="I","I",IF(LEFT(H75,1)="S","S",IF(LEFT(H75,1)="N","H",IF(LEFT(H75,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F75" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B75),",",H75," ",C75)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=811+S+CARROLL+ST,SLATER+IOWA</v>
-      </c>
-      <c r="G75" t="str">
-        <f>CONCATENATE(D75,"_",E75,"_",B75,".png")</f>
-        <v>G_S_ 811 S CARROLL ST .png</v>
+      <c r="F75" t="s">
+        <v>298</v>
+      </c>
+      <c r="G75" t="s">
+        <v>199</v>
       </c>
       <c r="H75" t="s">
         <v>30</v>
@@ -3000,16 +3446,14 @@
         <v>124</v>
       </c>
       <c r="E76" t="str">
-        <f>IF(LEFT(H76,1)="I","I",IF(LEFT(H76,1)="S","S",IF(LEFT(H76,1)="N","H",IF(LEFT(H76,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="F76" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B76),",",H76," ",C76)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=108+10TH+AVE,SLATER+IOWA</v>
-      </c>
-      <c r="G76" t="str">
-        <f>CONCATENATE(D76,"_",E76,"_",B76,".png")</f>
-        <v>G_S_ 108 10TH AVE .png</v>
+      <c r="F76" t="s">
+        <v>299</v>
+      </c>
+      <c r="G76" t="s">
+        <v>200</v>
       </c>
       <c r="H76" t="s">
         <v>30</v>
@@ -3029,16 +3473,14 @@
         <v>124</v>
       </c>
       <c r="E77" t="str">
-        <f>IF(LEFT(H77,1)="I","I",IF(LEFT(H77,1)="S","S",IF(LEFT(H77,1)="N","H",IF(LEFT(H77,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F77" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B77),",",H77," ",C77)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=303+I+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G77" t="str">
-        <f>CONCATENATE(D77,"_",E77,"_",B77,".png")</f>
-        <v>G_D_ 303 I AVE .png</v>
+      <c r="F77" t="s">
+        <v>300</v>
+      </c>
+      <c r="G77" t="s">
+        <v>201</v>
       </c>
       <c r="H77" t="s">
         <v>95</v>
@@ -3058,16 +3500,14 @@
         <v>124</v>
       </c>
       <c r="E78" t="str">
-        <f>IF(LEFT(H78,1)="I","I",IF(LEFT(H78,1)="S","S",IF(LEFT(H78,1)="N","H",IF(LEFT(H78,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F78" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B78),",",H78," ",C78)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=301+I+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G78" t="str">
-        <f>CONCATENATE(D78,"_",E78,"_",B78,".png")</f>
-        <v>G_D_ 301 I AVE .png</v>
+      <c r="F78" t="s">
+        <v>301</v>
+      </c>
+      <c r="G78" t="s">
+        <v>202</v>
       </c>
       <c r="H78" t="s">
         <v>95</v>
@@ -3087,16 +3527,14 @@
         <v>124</v>
       </c>
       <c r="E79" t="str">
-        <f>IF(LEFT(H79,1)="I","I",IF(LEFT(H79,1)="S","S",IF(LEFT(H79,1)="N","H",IF(LEFT(H79,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F79" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B79),",",H79," ",C79)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1206+4TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G79" t="str">
-        <f>CONCATENATE(D79,"_",E79,"_",B79,".png")</f>
-        <v>G_D_ 1206 4TH ST .png</v>
+      <c r="F79" t="s">
+        <v>302</v>
+      </c>
+      <c r="G79" t="s">
+        <v>203</v>
       </c>
       <c r="H79" t="s">
         <v>95</v>
@@ -3116,16 +3554,14 @@
         <v>124</v>
       </c>
       <c r="E80" t="str">
-        <f>IF(LEFT(H80,1)="I","I",IF(LEFT(H80,1)="S","S",IF(LEFT(H80,1)="N","H",IF(LEFT(H80,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F80" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B80),",",H80," ",C80)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=505+I+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G80" t="str">
-        <f>CONCATENATE(D80,"_",E80,"_",B80,".png")</f>
-        <v>G_D_ 505 I AVE .png</v>
+      <c r="F80" t="s">
+        <v>303</v>
+      </c>
+      <c r="G80" t="s">
+        <v>204</v>
       </c>
       <c r="H80" t="s">
         <v>95</v>
@@ -3145,16 +3581,14 @@
         <v>124</v>
       </c>
       <c r="E81" t="str">
-        <f>IF(LEFT(H81,1)="I","I",IF(LEFT(H81,1)="S","S",IF(LEFT(H81,1)="N","H",IF(LEFT(H81,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F81" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B81),",",H81," ",C81)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=212+K+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G81" t="str">
-        <f>CONCATENATE(D81,"_",E81,"_",B81,".png")</f>
-        <v>G_D_ 212 K AVE .png</v>
+      <c r="F81" t="s">
+        <v>304</v>
+      </c>
+      <c r="G81" t="s">
+        <v>205</v>
       </c>
       <c r="H81" t="s">
         <v>95</v>
@@ -3174,16 +3608,14 @@
         <v>124</v>
       </c>
       <c r="E82" t="str">
-        <f>IF(LEFT(H82,1)="I","I",IF(LEFT(H82,1)="S","S",IF(LEFT(H82,1)="N","H",IF(LEFT(H82,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F82" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B82),",",H82," ",C82)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1208+5TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G82" t="str">
-        <f>CONCATENATE(D82,"_",E82,"_",B82,".png")</f>
-        <v>G_D_ 1208 5TH ST .png</v>
+      <c r="F82" t="s">
+        <v>305</v>
+      </c>
+      <c r="G82" t="s">
+        <v>206</v>
       </c>
       <c r="H82" t="s">
         <v>95</v>
@@ -3203,16 +3635,14 @@
         <v>124</v>
       </c>
       <c r="E83" t="str">
-        <f>IF(LEFT(H83,1)="I","I",IF(LEFT(H83,1)="S","S",IF(LEFT(H83,1)="N","H",IF(LEFT(H83,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F83" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B83),",",H83," ",C83)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=808+FROST+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G83" t="str">
-        <f>CONCATENATE(D83,"_",E83,"_",B83,".png")</f>
-        <v>G_D_ 808 FROST ST .png</v>
+      <c r="F83" t="s">
+        <v>306</v>
+      </c>
+      <c r="G83" t="s">
+        <v>207</v>
       </c>
       <c r="H83" t="s">
         <v>95</v>
@@ -3232,16 +3662,14 @@
         <v>124</v>
       </c>
       <c r="E84" t="str">
-        <f>IF(LEFT(H84,1)="I","I",IF(LEFT(H84,1)="S","S",IF(LEFT(H84,1)="N","H",IF(LEFT(H84,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F84" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B84),",",H84," ",C84)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=307+I+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G84" t="str">
-        <f>CONCATENATE(D84,"_",E84,"_",B84,".png")</f>
-        <v>G_D_ 307 I AVE .png</v>
+      <c r="F84" t="s">
+        <v>307</v>
+      </c>
+      <c r="G84" t="s">
+        <v>208</v>
       </c>
       <c r="H84" t="s">
         <v>95</v>
@@ -3261,16 +3689,14 @@
         <v>124</v>
       </c>
       <c r="E85" t="str">
-        <f>IF(LEFT(H85,1)="I","I",IF(LEFT(H85,1)="S","S",IF(LEFT(H85,1)="N","H",IF(LEFT(H85,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F85" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B85),",",H85," ",C85)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=310+E+M+Ave,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G85" t="str">
-        <f>CONCATENATE(D85,"_",E85,"_",B85,".png")</f>
-        <v>G_D_ 310 E M Ave.png</v>
+      <c r="F85" t="s">
+        <v>308</v>
+      </c>
+      <c r="G85" t="s">
+        <v>209</v>
       </c>
       <c r="H85" t="s">
         <v>95</v>
@@ -3290,16 +3716,14 @@
         <v>124</v>
       </c>
       <c r="E86" t="str">
-        <f>IF(LEFT(H86,1)="I","I",IF(LEFT(H86,1)="S","S",IF(LEFT(H86,1)="N","H",IF(LEFT(H86,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F86" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B86),",",H86," ",C86)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=501+HYDE+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G86" t="str">
-        <f>CONCATENATE(D86,"_",E86,"_",B86,".png")</f>
-        <v>G_D_ 501 HYDE AVE .png</v>
+      <c r="F86" t="s">
+        <v>309</v>
+      </c>
+      <c r="G86" t="s">
+        <v>210</v>
       </c>
       <c r="H86" t="s">
         <v>95</v>
@@ -3319,16 +3743,14 @@
         <v>124</v>
       </c>
       <c r="E87" t="str">
-        <f>IF(LEFT(H87,1)="I","I",IF(LEFT(H87,1)="S","S",IF(LEFT(H87,1)="N","H",IF(LEFT(H87,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F87" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B87),",",H87," ",C87)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=302+H+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G87" t="str">
-        <f>CONCATENATE(D87,"_",E87,"_",B87,".png")</f>
-        <v>G_D_ 302 H AVE .png</v>
+      <c r="F87" t="s">
+        <v>310</v>
+      </c>
+      <c r="G87" t="s">
+        <v>211</v>
       </c>
       <c r="H87" t="s">
         <v>95</v>
@@ -3348,16 +3770,14 @@
         <v>124</v>
       </c>
       <c r="E88" t="str">
-        <f>IF(LEFT(H88,1)="I","I",IF(LEFT(H88,1)="S","S",IF(LEFT(H88,1)="N","H",IF(LEFT(H88,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F88" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B88),",",H88," ",C88)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=314+H+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G88" t="str">
-        <f>CONCATENATE(D88,"_",E88,"_",B88,".png")</f>
-        <v>G_D_ 314 H AVE .png</v>
+      <c r="F88" t="s">
+        <v>311</v>
+      </c>
+      <c r="G88" t="s">
+        <v>212</v>
       </c>
       <c r="H88" t="s">
         <v>95</v>
@@ -3377,16 +3797,14 @@
         <v>124</v>
       </c>
       <c r="E89" t="str">
-        <f>IF(LEFT(H89,1)="I","I",IF(LEFT(H89,1)="S","S",IF(LEFT(H89,1)="N","H",IF(LEFT(H89,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F89" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B89),",",H89," ",C89)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=411+Hyde+Ave,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G89" t="str">
-        <f>CONCATENATE(D89,"_",E89,"_",B89,".png")</f>
-        <v>G_D_ 411 Hyde Ave.png</v>
+      <c r="F89" t="s">
+        <v>312</v>
+      </c>
+      <c r="G89" t="s">
+        <v>213</v>
       </c>
       <c r="H89" t="s">
         <v>95</v>
@@ -3406,16 +3824,14 @@
         <v>124</v>
       </c>
       <c r="E90" t="str">
-        <f>IF(LEFT(H90,1)="I","I",IF(LEFT(H90,1)="S","S",IF(LEFT(H90,1)="N","H",IF(LEFT(H90,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F90" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B90),",",H90," ",C90)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=403+H+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G90" t="str">
-        <f>CONCATENATE(D90,"_",E90,"_",B90,".png")</f>
-        <v>G_D_ 403 H AVE .png</v>
+      <c r="F90" t="s">
+        <v>313</v>
+      </c>
+      <c r="G90" t="s">
+        <v>214</v>
       </c>
       <c r="H90" t="s">
         <v>95</v>
@@ -3435,16 +3851,14 @@
         <v>124</v>
       </c>
       <c r="E91" t="str">
-        <f>IF(LEFT(H91,1)="I","I",IF(LEFT(H91,1)="S","S",IF(LEFT(H91,1)="N","H",IF(LEFT(H91,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F91" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B91),",",H91," ",C91)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=708+5TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G91" t="str">
-        <f>CONCATENATE(D91,"_",E91,"_",B91,".png")</f>
-        <v>G_D_ 708 5TH ST .png</v>
+      <c r="F91" t="s">
+        <v>314</v>
+      </c>
+      <c r="G91" t="s">
+        <v>215</v>
       </c>
       <c r="H91" t="s">
         <v>95</v>
@@ -3464,16 +3878,14 @@
         <v>124</v>
       </c>
       <c r="E92" t="str">
-        <f>IF(LEFT(H92,1)="I","I",IF(LEFT(H92,1)="S","S",IF(LEFT(H92,1)="N","H",IF(LEFT(H92,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F92" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B92),",",H92," ",C92)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=302+E+H+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G92" t="str">
-        <f>CONCATENATE(D92,"_",E92,"_",B92,".png")</f>
-        <v>G_D_ 302 E H AVE .png</v>
+      <c r="F92" t="s">
+        <v>315</v>
+      </c>
+      <c r="G92" t="s">
+        <v>216</v>
       </c>
       <c r="H92" t="s">
         <v>95</v>
@@ -3493,16 +3905,14 @@
         <v>124</v>
       </c>
       <c r="E93" t="str">
-        <f>IF(LEFT(H93,1)="I","I",IF(LEFT(H93,1)="S","S",IF(LEFT(H93,1)="N","H",IF(LEFT(H93,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F93" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B93),",",H93," ",C93)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=310+G+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G93" t="str">
-        <f>CONCATENATE(D93,"_",E93,"_",B93,".png")</f>
-        <v>G_D_ 310 G AVE .png</v>
+      <c r="F93" t="s">
+        <v>316</v>
+      </c>
+      <c r="G93" t="s">
+        <v>217</v>
       </c>
       <c r="H93" t="s">
         <v>95</v>
@@ -3522,16 +3932,14 @@
         <v>124</v>
       </c>
       <c r="E94" t="str">
-        <f>IF(LEFT(H94,1)="I","I",IF(LEFT(H94,1)="S","S",IF(LEFT(H94,1)="N","H",IF(LEFT(H94,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F94" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B94),",",H94," ",C94)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1204+4TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G94" t="str">
-        <f>CONCATENATE(D94,"_",E94,"_",B94,".png")</f>
-        <v>G_D_ 1204 4TH ST .png</v>
+      <c r="F94" t="s">
+        <v>317</v>
+      </c>
+      <c r="G94" t="s">
+        <v>218</v>
       </c>
       <c r="H94" t="s">
         <v>95</v>
@@ -3551,16 +3959,14 @@
         <v>124</v>
       </c>
       <c r="E95" t="str">
-        <f>IF(LEFT(H95,1)="I","I",IF(LEFT(H95,1)="S","S",IF(LEFT(H95,1)="N","H",IF(LEFT(H95,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F95" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B95),",",H95," ",C95)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1202+4TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G95" t="str">
-        <f>CONCATENATE(D95,"_",E95,"_",B95,".png")</f>
-        <v>G_D_ 1202 4TH ST .png</v>
+      <c r="F95" t="s">
+        <v>318</v>
+      </c>
+      <c r="G95" t="s">
+        <v>219</v>
       </c>
       <c r="H95" t="s">
         <v>95</v>
@@ -3580,16 +3986,14 @@
         <v>124</v>
       </c>
       <c r="E96" t="str">
-        <f>IF(LEFT(H96,1)="I","I",IF(LEFT(H96,1)="S","S",IF(LEFT(H96,1)="N","H",IF(LEFT(H96,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F96" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B96),",",H96," ",C96)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=803+FROST+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G96" t="str">
-        <f>CONCATENATE(D96,"_",E96,"_",B96,".png")</f>
-        <v>G_D_ 803 FROST ST .png</v>
+      <c r="F96" t="s">
+        <v>319</v>
+      </c>
+      <c r="G96" t="s">
+        <v>220</v>
       </c>
       <c r="H96" t="s">
         <v>95</v>
@@ -3609,16 +4013,14 @@
         <v>124</v>
       </c>
       <c r="E97" t="str">
-        <f>IF(LEFT(H97,1)="I","I",IF(LEFT(H97,1)="S","S",IF(LEFT(H97,1)="N","H",IF(LEFT(H97,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F97" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B97),",",H97," ",C97)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=1104+4TH+ST,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G97" t="str">
-        <f>CONCATENATE(D97,"_",E97,"_",B97,".png")</f>
-        <v>G_D_ 1104 4TH ST .png</v>
+      <c r="F97" t="s">
+        <v>320</v>
+      </c>
+      <c r="G97" t="s">
+        <v>221</v>
       </c>
       <c r="H97" t="s">
         <v>95</v>
@@ -3638,16 +4040,14 @@
         <v>124</v>
       </c>
       <c r="E98" t="str">
-        <f>IF(LEFT(H98,1)="I","I",IF(LEFT(H98,1)="S","S",IF(LEFT(H98,1)="N","H",IF(LEFT(H98,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F98" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B98),",",H98," ",C98)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=212+J+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G98" t="str">
-        <f>CONCATENATE(D98,"_",E98,"_",B98,".png")</f>
-        <v>G_D_ 212 J AVE .png</v>
+      <c r="F98" t="s">
+        <v>321</v>
+      </c>
+      <c r="G98" t="s">
+        <v>222</v>
       </c>
       <c r="H98" t="s">
         <v>95</v>
@@ -3667,16 +4067,14 @@
         <v>124</v>
       </c>
       <c r="E99" t="str">
-        <f>IF(LEFT(H99,1)="I","I",IF(LEFT(H99,1)="S","S",IF(LEFT(H99,1)="N","H",IF(LEFT(H99,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F99" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B99),",",H99," ",C99)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=202+K+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G99" t="str">
-        <f>CONCATENATE(D99,"_",E99,"_",B99,".png")</f>
-        <v>G_D_ 202 K AVE .png</v>
+      <c r="F99" t="s">
+        <v>322</v>
+      </c>
+      <c r="G99" t="s">
+        <v>223</v>
       </c>
       <c r="H99" t="s">
         <v>95</v>
@@ -3696,16 +4094,14 @@
         <v>124</v>
       </c>
       <c r="E100" t="str">
-        <f>IF(LEFT(H100,1)="I","I",IF(LEFT(H100,1)="S","S",IF(LEFT(H100,1)="N","H",IF(LEFT(H100,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F100" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B100),",",H100," ",C100)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=313+H+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G100" t="str">
-        <f>CONCATENATE(D100,"_",E100,"_",B100,".png")</f>
-        <v>G_D_ 313 H AVE .png</v>
+      <c r="F100" t="s">
+        <v>323</v>
+      </c>
+      <c r="G100" t="s">
+        <v>224</v>
       </c>
       <c r="H100" t="s">
         <v>95</v>
@@ -3725,16 +4121,14 @@
         <v>124</v>
       </c>
       <c r="E101" t="str">
-        <f>IF(LEFT(H101,1)="I","I",IF(LEFT(H101,1)="S","S",IF(LEFT(H101,1)="N","H",IF(LEFT(H101,1)="G","D"))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="F101" t="str">
-        <f>SUBSTITUTE(CONCATENATE("https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=",TRIM(B101),",",H101," ",C101)," ","+")</f>
-        <v>https://maps.googleapis.com/maps/api/streetview?size=800x800&amp;location=502+BUTLER+AVE,GRUNDY+CENTER+IOWA</v>
-      </c>
-      <c r="G101" t="str">
-        <f>CONCATENATE(D101,"_",E101,"_",B101,".png")</f>
-        <v>G_D_ 502 BUTLER AVE .png</v>
+      <c r="F101" t="s">
+        <v>324</v>
+      </c>
+      <c r="G101" t="s">
+        <v>225</v>
       </c>
       <c r="H101" t="s">
         <v>95</v>

</xml_diff>